<commit_message>
add Item Recovery and Armer
</commit_message>
<xml_diff>
--- a/MySurvivorsGame/Assets/StreamingAssets/ItemData.xlsx
+++ b/MySurvivorsGame/Assets/StreamingAssets/ItemData.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="46">
   <si>
     <t>ItemName</t>
   </si>
@@ -77,7 +77,7 @@
     <t>Assets/ArtResources/Items/Armer.png</t>
   </si>
   <si>
-    <t>被害軽減</t>
+    <t>ダメージ軽減</t>
   </si>
   <si>
     <t>Attack</t>
@@ -183,12 +183,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9900"/>
+        <bgColor rgb="FFFF9900"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -203,9 +209,18 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
@@ -214,12 +229,9 @@
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment horizontal="left" readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -497,190 +509,190 @@
       <c r="G1" s="3"/>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="4" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="3"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="5" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="C4" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="E4" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="1" t="s">
+      <c r="F4" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G4" s="3"/>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D5" s="4" t="s">
+      <c r="C5" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="5" t="s">
+      <c r="E5" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="4" t="s">
+      <c r="F5" s="6" t="s">
         <v>19</v>
       </c>
       <c r="G5" s="3"/>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="E6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>22</v>
       </c>
       <c r="G6" s="3"/>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D7" s="4" t="s">
+      <c r="C7" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="E7" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F7" s="4" t="s">
+      <c r="F7" s="6" t="s">
         <v>25</v>
       </c>
       <c r="G7" s="3"/>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="C8" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="6" t="s">
         <v>28</v>
       </c>
       <c r="G8" s="3"/>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B9" s="4" t="s">
+      <c r="B9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E9" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="6" t="s">
         <v>31</v>
       </c>
       <c r="G9" s="3"/>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B10" s="4" t="s">
+      <c r="B10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C10" s="1">
-        <v>0.0</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="4" t="s">
+      <c r="E10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="4" t="s">
+      <c r="F10" s="6" t="s">
         <v>34</v>
       </c>
     </row>
@@ -700,66 +712,66 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1.0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>2.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>4.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>3.0</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>8.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>16.0</v>
       </c>
     </row>
@@ -779,66 +791,64 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="B1" s="1" t="s">
+      <c r="A1" s="5"/>
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1.0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>1.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>3.0</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>3.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>4.0</v>
       </c>
     </row>
@@ -858,66 +868,66 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1.0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>1.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>3.0</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>4.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>10.0</v>
       </c>
     </row>
@@ -937,66 +947,66 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1.0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>1.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>3.0</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>4.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>6.0</v>
       </c>
     </row>
@@ -1016,66 +1026,66 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1.0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>1.5</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>2.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>3.0</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>4.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>6.0</v>
       </c>
     </row>
@@ -1095,67 +1105,67 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="6">
         <v>0.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1.0</v>
       </c>
-      <c r="B5" s="4">
-        <v>40.0</v>
+      <c r="B5" s="6">
+        <v>50.0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4">
-        <v>80.0</v>
+      <c r="B6" s="6">
+        <v>100.0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>3.0</v>
       </c>
-      <c r="B7" s="4">
-        <v>160.0</v>
+      <c r="B7" s="6">
+        <v>200.0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
-        <v>320.0</v>
+      <c r="B8" s="6">
+        <v>400.0</v>
       </c>
     </row>
   </sheetData>
@@ -1174,66 +1184,66 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="4">
-        <v>0.0</v>
-      </c>
-      <c r="B4" s="4">
+      <c r="A4" s="6">
+        <v>0.0</v>
+      </c>
+      <c r="B4" s="6">
         <v>1.0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="4">
+      <c r="A5" s="6">
         <v>1.0</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="6">
         <v>1.1</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="4">
+      <c r="A6" s="6">
         <v>2.0</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="6">
         <v>1.2</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="4">
+      <c r="A7" s="6">
         <v>3.0</v>
       </c>
-      <c r="B7" s="4">
+      <c r="B7" s="6">
         <v>1.3</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="4">
+      <c r="A8" s="6">
         <v>4.0</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="6">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>